<commit_message>
changelist: command tests improved exception handling rebuilt exception signatures admin commands bugs fixed:  saving admin self giving item  saving admin self teleporting failing fast on item script mapping failure
</commit_message>
<xml_diff>
--- a/mainCity.xlsx
+++ b/mainCity.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="19">
   <si>
     <t>Opuszczony dom</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Karczma</t>
+  </si>
+  <si>
+    <t>Skrzyżowanie Aleji Bocznej i Przemysłowej</t>
   </si>
 </sst>
 </file>
@@ -650,7 +653,7 @@
   <dimension ref="G11:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="53.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -739,7 +742,7 @@
         <v>16</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>3</v>

</xml_diff>